<commit_message>
update import data relasi
</commit_message>
<xml_diff>
--- a/public/SoalData/soaldata.xlsx
+++ b/public/SoalData/soaldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF5112C-CE00-46F9-B579-9D36772BB2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F46116-34F9-4BC6-B808-8E91FE3D0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9D0E831C-A0F9-45CE-95D6-7A6BF3FF0510}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TANGKAI : KELOPAK : BUNGA=</t>
   </si>
@@ -34,6 +34,51 @@
   </si>
   <si>
     <t>Perbandingan kelereng Egi dan Legi adalah 3 : 2. Jika selisih kelereng mereka 8, jumlah kelereng Egi dan Legi adalah…</t>
+  </si>
+  <si>
+    <t>A. Tubuh : tangan : kepala</t>
+  </si>
+  <si>
+    <t>B. Tanah : laut : air</t>
+  </si>
+  <si>
+    <t>C. Tahun : bulan : hari</t>
+  </si>
+  <si>
+    <t>D. Pelepah : tangkai : daun</t>
+  </si>
+  <si>
+    <t>E. Langit : tanah : magma</t>
+  </si>
+  <si>
+    <t>A. K dan J</t>
+  </si>
+  <si>
+    <t>B. J dan K</t>
+  </si>
+  <si>
+    <t>C. M dan N</t>
+  </si>
+  <si>
+    <t>D. N dan M</t>
+  </si>
+  <si>
+    <t>E. I dan H</t>
+  </si>
+  <si>
+    <t>A. 40</t>
+  </si>
+  <si>
+    <t>B. 32</t>
+  </si>
+  <si>
+    <t>C. 24</t>
+  </si>
+  <si>
+    <t>D. 16</t>
+  </si>
+  <si>
+    <t>E. 25</t>
   </si>
 </sst>
 </file>
@@ -73,7 +118,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,52 +434,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C122ED9-E99B-43E2-BF27-D3B6F5088175}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="105.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>50</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>6</v>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>